<commit_message>
Tests: Fix YAML generation and schema validation tests
</commit_message>
<xml_diff>
--- a/tests/metadata-generation/fixtures/botek.xlsx
+++ b/tests/metadata-generation/fixtures/botek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\tests\metadata-generation\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CEF3C6-D30B-4172-A514-2BD4A2111C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF69D727-89B6-4975-8AED-CC898D45A379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="755" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="178">
   <si>
     <t>Person</t>
   </si>
@@ -286,9 +286,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -328,9 +325,6 @@
     <t>Drilling</t>
   </si>
   <si>
-    <t>file</t>
-  </si>
-  <si>
     <t>files</t>
   </si>
   <si>
@@ -659,6 +653,15 @@
   </si>
   <si>
     <t xml:space="preserve">Max. Wear at Tool Tip </t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>float_qty</t>
+  </si>
+  <si>
+    <t>int_qty</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1189,7 +1192,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>28</v>
@@ -1262,7 +1265,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>30</v>
@@ -1273,16 +1276,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -1290,13 +1293,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -1307,16 +1310,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>33</v>
@@ -1324,13 +1327,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>32</v>
@@ -1341,10 +1344,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>28</v>
@@ -1355,10 +1358,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>28</v>
@@ -1369,10 +1372,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>29</v>
@@ -1383,10 +1386,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>29</v>
@@ -1403,7 +1406,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>32</v>
@@ -1414,13 +1417,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>32</v>
@@ -1431,13 +1434,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>32</v>
@@ -1448,10 +1451,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
@@ -1478,10 +1481,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>29</v>
@@ -1508,16 +1511,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>34</v>
@@ -1525,13 +1528,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>175</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>34</v>
@@ -1539,13 +1542,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>34</v>
@@ -1553,13 +1556,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>34</v>
@@ -1567,13 +1570,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>34</v>
@@ -1581,13 +1584,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>32</v>
@@ -1598,13 +1601,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>32</v>
@@ -1615,16 +1618,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>34</v>
@@ -1632,10 +1635,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>51</v>
@@ -1646,16 +1649,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>34</v>
@@ -1663,16 +1666,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>34</v>
@@ -1680,16 +1683,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>34</v>
@@ -1697,13 +1700,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
@@ -1712,16 +1715,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>34</v>
@@ -1729,13 +1732,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>175</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="3" t="s">
@@ -1744,10 +1747,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>51</v>
@@ -1768,7 +1771,7 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
@@ -1783,7 +1786,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1866,50 +1869,50 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1947,13 +1950,13 @@
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1964,16 +1967,16 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -1981,16 +1984,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2001,42 +2004,42 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2059,7 +2062,7 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -2090,7 +2093,7 @@
         <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -2098,7 +2101,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2106,7 +2109,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -2115,7 +2118,7 @@
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -2129,7 +2132,7 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -2143,10 +2146,10 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -2160,7 +2163,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -2174,7 +2177,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -2188,35 +2191,35 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
@@ -2227,57 +2230,57 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
         <v>163</v>
-      </c>
-      <c r="E13" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -2288,18 +2291,18 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
@@ -2315,7 +2318,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -2337,7 +2340,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2348,7 +2351,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -2359,7 +2362,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -2370,7 +2373,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -2392,7 +2395,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -2465,7 +2468,7 @@
         <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -2473,7 +2476,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2481,7 +2484,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -2490,179 +2493,179 @@
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
         <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2721,7 +2724,7 @@
         <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -2729,7 +2732,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2737,7 +2740,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -2746,7 +2749,7 @@
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -2760,7 +2763,7 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -2774,10 +2777,10 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -2791,7 +2794,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -2805,7 +2808,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -2819,35 +2822,35 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
@@ -2858,57 +2861,57 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
         <v>163</v>
-      </c>
-      <c r="E13" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
@@ -2919,18 +2922,18 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -2946,7 +2949,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -2968,7 +2971,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2979,7 +2982,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -2990,7 +2993,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -3001,7 +3004,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -3023,7 +3026,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -3034,7 +3037,7 @@
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>1</v>
@@ -3043,12 +3046,12 @@
         <v>18</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>1</v>
@@ -3060,7 +3063,7 @@
     </row>
     <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>1</v>
@@ -3069,7 +3072,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
@@ -3180,7 +3183,7 @@
         <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3188,7 +3191,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3196,7 +3199,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -3205,179 +3208,179 @@
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
         <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">

</xml_diff>